<commit_message>
updata result of denoise
</commit_message>
<xml_diff>
--- a/v5/main_exp/regression_cov_orth.xlsx
+++ b/v5/main_exp/regression_cov_orth.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\master\ensemble_github\experimental_data\v5\main_exp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCD6141-49B6-4593-B28F-527C565D9B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5E8AAE-C610-451B-9131-096E2D2FD1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6900" yWindow="5450" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -817,9 +817,6 @@
     <t>-7.90%</t>
   </si>
   <si>
-    <t>concrete_compressive_strength:regression</t>
-  </si>
-  <si>
     <t>4.8096,(0.00%:6)</t>
   </si>
   <si>
@@ -1670,9 +1667,6 @@
   </si>
   <si>
     <t>-5.93%</t>
-  </si>
-  <si>
-    <t>yacht_hydrodynamics:regression</t>
   </si>
   <si>
     <t>3.7701,(0.00%:8)</t>
@@ -3213,6 +3207,14 @@
   </si>
   <si>
     <t>elevators:regression</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>yacht_hydrodynamics:regression</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>concrete_compressive_strength:regression</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -3232,18 +3234,21 @@
       <b/>
       <sz val="11"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -3601,8 +3606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
@@ -4671,34 +4676,34 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>265</v>
+        <v>1063</v>
       </c>
       <c r="B34" t="s">
         <v>11</v>
       </c>
       <c r="C34" t="s">
+        <v>265</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="E34" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="F34" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="G34" s="2" t="s">
         <v>269</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="H34" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="I34" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="I34" s="2" t="s">
+      <c r="J34" s="2" t="s">
         <v>272</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
@@ -4709,28 +4714,28 @@
         <v>21</v>
       </c>
       <c r="C35" t="s">
+        <v>273</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="E35" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="F35" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="G35" s="2" t="s">
+      <c r="H35" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="I35" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="I35" s="2" t="s">
+      <c r="J35" s="2" t="s">
         <v>280</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
@@ -4741,28 +4746,28 @@
         <v>30</v>
       </c>
       <c r="C36" t="s">
+        <v>281</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="E36" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="F36" s="2" t="s">
         <v>284</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="G36" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="H36" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="H36" s="2" t="s">
+      <c r="I36" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="I36" s="2" t="s">
+      <c r="J36" s="2" t="s">
         <v>288</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
@@ -4773,28 +4778,28 @@
         <v>39</v>
       </c>
       <c r="C37" t="s">
+        <v>289</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="E37" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="F37" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="G37" s="2" t="s">
         <v>293</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="H37" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="H37" s="2" t="s">
+      <c r="I37" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="I37" s="2" t="s">
+      <c r="J37" s="2" t="s">
         <v>296</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
@@ -4805,28 +4810,28 @@
         <v>48</v>
       </c>
       <c r="C38" t="s">
+        <v>297</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="E38" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="F38" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="G38" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="G38" s="2" t="s">
+      <c r="H38" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="H38" s="2" t="s">
+      <c r="I38" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="I38" s="2" t="s">
+      <c r="J38" s="2" t="s">
         <v>304</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -4837,28 +4842,28 @@
         <v>57</v>
       </c>
       <c r="C39" t="s">
+        <v>305</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="F39" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="G39" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="H39" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="H39" s="2" t="s">
+      <c r="I39" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="I39" s="2" t="s">
+      <c r="J39" s="2" t="s">
         <v>312</v>
-      </c>
-      <c r="J39" s="2" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
@@ -4869,16 +4874,16 @@
         <v>66</v>
       </c>
       <c r="C40" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D40" t="s">
         <v>132</v>
       </c>
       <c r="E40" t="s">
+        <v>314</v>
+      </c>
+      <c r="F40" t="s">
         <v>315</v>
-      </c>
-      <c r="F40" t="s">
-        <v>316</v>
       </c>
       <c r="G40" t="s">
         <v>257</v>
@@ -4887,7 +4892,7 @@
         <v>71</v>
       </c>
       <c r="I40" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="J40" t="s">
         <v>256</v>
@@ -4904,57 +4909,57 @@
         <v>74</v>
       </c>
       <c r="D41" t="s">
+        <v>317</v>
+      </c>
+      <c r="E41" t="s">
         <v>318</v>
       </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
         <v>319</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>320</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>321</v>
       </c>
-      <c r="H41" t="s">
+      <c r="I41" t="s">
         <v>322</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
         <v>323</v>
-      </c>
-      <c r="J41" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="B42" t="s">
         <v>11</v>
       </c>
       <c r="C42" t="s">
+        <v>324</v>
+      </c>
+      <c r="D42" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="F42" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="G42" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="H42" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="I42" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="I42" s="3" t="s">
+      <c r="J42" s="3" t="s">
         <v>331</v>
-      </c>
-      <c r="J42" s="3" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -4965,28 +4970,28 @@
         <v>21</v>
       </c>
       <c r="C43" t="s">
+        <v>332</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="G43" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="H43" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="H43" s="2" t="s">
+      <c r="I43" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="I43" s="2" t="s">
+      <c r="J43" s="2" t="s">
         <v>339</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -4997,28 +5002,28 @@
         <v>30</v>
       </c>
       <c r="C44" t="s">
+        <v>340</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="G44" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="H44" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="I44" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="I44" s="2" t="s">
+      <c r="J44" s="2" t="s">
         <v>347</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -5029,28 +5034,28 @@
         <v>39</v>
       </c>
       <c r="C45" t="s">
+        <v>348</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="E45" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="F45" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="G45" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="H45" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="H45" s="2" t="s">
+      <c r="I45" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="I45" s="2" t="s">
+      <c r="J45" s="2" t="s">
         <v>355</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -5061,28 +5066,28 @@
         <v>48</v>
       </c>
       <c r="C46" t="s">
+        <v>356</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="E46" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="F46" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="G46" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="H46" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="H46" s="2" t="s">
+      <c r="I46" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="I46" s="2" t="s">
+      <c r="J46" s="2" t="s">
         <v>363</v>
-      </c>
-      <c r="J46" s="2" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -5093,28 +5098,28 @@
         <v>57</v>
       </c>
       <c r="C47" t="s">
+        <v>364</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="E47" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="F47" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="G47" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="H47" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="H47" s="2" t="s">
+      <c r="I47" s="2" t="s">
         <v>370</v>
       </c>
-      <c r="I47" s="2" t="s">
+      <c r="J47" s="2" t="s">
         <v>371</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
@@ -5125,25 +5130,25 @@
         <v>66</v>
       </c>
       <c r="C48" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D48" t="s">
         <v>196</v>
       </c>
       <c r="E48" t="s">
+        <v>372</v>
+      </c>
+      <c r="F48" t="s">
         <v>373</v>
       </c>
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>374</v>
-      </c>
-      <c r="G48" t="s">
-        <v>375</v>
       </c>
       <c r="H48" t="s">
         <v>195</v>
       </c>
       <c r="I48" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="J48" t="s">
         <v>256</v>
@@ -5160,57 +5165,57 @@
         <v>74</v>
       </c>
       <c r="D49" t="s">
+        <v>376</v>
+      </c>
+      <c r="E49" t="s">
         <v>377</v>
       </c>
-      <c r="E49" t="s">
+      <c r="F49" t="s">
         <v>378</v>
       </c>
-      <c r="F49" t="s">
+      <c r="G49" t="s">
         <v>379</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
+        <v>320</v>
+      </c>
+      <c r="I49" t="s">
         <v>380</v>
       </c>
-      <c r="H49" t="s">
-        <v>321</v>
-      </c>
-      <c r="I49" t="s">
+      <c r="J49" t="s">
         <v>381</v>
-      </c>
-      <c r="J49" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="B50" t="s">
         <v>11</v>
       </c>
       <c r="C50" t="s">
+        <v>382</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>383</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="E50" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="F50" s="2" t="s">
         <v>385</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="G50" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="G50" s="3" t="s">
+      <c r="H50" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="H50" s="3" t="s">
+      <c r="I50" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="I50" s="3" t="s">
+      <c r="J50" s="3" t="s">
         <v>389</v>
-      </c>
-      <c r="J50" s="3" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
@@ -5221,28 +5226,28 @@
         <v>21</v>
       </c>
       <c r="C51" t="s">
+        <v>390</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="E51" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="F51" s="2" t="s">
         <v>393</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="G51" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="G51" s="3" t="s">
+      <c r="H51" s="2" t="s">
         <v>395</v>
       </c>
-      <c r="H51" s="2" t="s">
+      <c r="I51" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="I51" s="2" t="s">
+      <c r="J51" s="2" t="s">
         <v>397</v>
-      </c>
-      <c r="J51" s="2" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
@@ -5253,28 +5258,28 @@
         <v>30</v>
       </c>
       <c r="C52" t="s">
+        <v>398</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>399</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="E52" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="F52" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="G52" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="G52" s="2" t="s">
+      <c r="H52" s="2" t="s">
         <v>403</v>
       </c>
-      <c r="H52" s="2" t="s">
+      <c r="I52" s="2" t="s">
         <v>404</v>
       </c>
-      <c r="I52" s="2" t="s">
+      <c r="J52" s="2" t="s">
         <v>405</v>
-      </c>
-      <c r="J52" s="2" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -5285,28 +5290,28 @@
         <v>39</v>
       </c>
       <c r="C53" t="s">
+        <v>406</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="E53" s="2" t="s">
         <v>408</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="F53" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="G53" s="2" t="s">
         <v>410</v>
       </c>
-      <c r="G53" s="2" t="s">
+      <c r="H53" s="2" t="s">
         <v>411</v>
       </c>
-      <c r="H53" s="2" t="s">
+      <c r="I53" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="I53" s="2" t="s">
+      <c r="J53" s="2" t="s">
         <v>413</v>
-      </c>
-      <c r="J53" s="2" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
@@ -5317,28 +5322,28 @@
         <v>48</v>
       </c>
       <c r="C54" t="s">
+        <v>414</v>
+      </c>
+      <c r="D54" s="2" t="s">
         <v>415</v>
       </c>
-      <c r="D54" s="2" t="s">
+      <c r="E54" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="F54" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="F54" s="2" t="s">
+      <c r="G54" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="G54" s="2" t="s">
+      <c r="H54" s="2" t="s">
         <v>419</v>
       </c>
-      <c r="H54" s="2" t="s">
+      <c r="I54" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="I54" s="2" t="s">
+      <c r="J54" s="2" t="s">
         <v>421</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
@@ -5349,28 +5354,28 @@
         <v>57</v>
       </c>
       <c r="C55" t="s">
+        <v>422</v>
+      </c>
+      <c r="D55" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="D55" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="F55" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="F55" s="2" t="s">
+      <c r="G55" s="2" t="s">
         <v>426</v>
       </c>
-      <c r="G55" s="2" t="s">
+      <c r="H55" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="H55" s="2" t="s">
+      <c r="I55" s="2" t="s">
         <v>428</v>
       </c>
-      <c r="I55" s="2" t="s">
+      <c r="J55" s="2" t="s">
         <v>429</v>
-      </c>
-      <c r="J55" s="2" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -5393,7 +5398,7 @@
         <v>194</v>
       </c>
       <c r="G56" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H56" t="s">
         <v>71</v>
@@ -5422,51 +5427,51 @@
         <v>139</v>
       </c>
       <c r="F57" t="s">
+        <v>431</v>
+      </c>
+      <c r="G57" t="s">
         <v>432</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>433</v>
       </c>
-      <c r="H57" t="s">
+      <c r="I57" t="s">
         <v>434</v>
       </c>
-      <c r="I57" t="s">
+      <c r="J57" t="s">
         <v>435</v>
-      </c>
-      <c r="J57" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B58" t="s">
         <v>11</v>
       </c>
       <c r="C58" t="s">
+        <v>437</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="D58" s="3" t="s">
+      <c r="E58" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="F58" s="3" t="s">
         <v>440</v>
       </c>
-      <c r="F58" s="3" t="s">
+      <c r="G58" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="G58" s="3" t="s">
+      <c r="H58" s="3" t="s">
         <v>442</v>
       </c>
-      <c r="H58" s="3" t="s">
+      <c r="I58" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="I58" s="3" t="s">
+      <c r="J58" s="3" t="s">
         <v>444</v>
-      </c>
-      <c r="J58" s="3" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
@@ -5477,28 +5482,28 @@
         <v>21</v>
       </c>
       <c r="C59" t="s">
+        <v>445</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="E59" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="E59" s="2" t="s">
+      <c r="F59" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="G59" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="G59" s="3" t="s">
+      <c r="H59" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="H59" s="2" t="s">
+      <c r="I59" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="I59" s="3" t="s">
+      <c r="J59" s="2" t="s">
         <v>452</v>
-      </c>
-      <c r="J59" s="2" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
@@ -5509,28 +5514,28 @@
         <v>30</v>
       </c>
       <c r="C60" t="s">
+        <v>453</v>
+      </c>
+      <c r="D60" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="D60" s="3" t="s">
+      <c r="E60" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="F60" s="3" t="s">
         <v>456</v>
       </c>
-      <c r="F60" s="3" t="s">
+      <c r="G60" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="G60" s="3" t="s">
+      <c r="H60" s="3" t="s">
         <v>458</v>
       </c>
-      <c r="H60" s="3" t="s">
+      <c r="I60" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="I60" s="3" t="s">
+      <c r="J60" s="3" t="s">
         <v>460</v>
-      </c>
-      <c r="J60" s="3" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
@@ -5541,28 +5546,28 @@
         <v>39</v>
       </c>
       <c r="C61" t="s">
+        <v>461</v>
+      </c>
+      <c r="D61" s="3" t="s">
         <v>462</v>
       </c>
-      <c r="D61" s="3" t="s">
+      <c r="E61" s="3" t="s">
         <v>463</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="F61" s="3" t="s">
         <v>464</v>
       </c>
-      <c r="F61" s="3" t="s">
+      <c r="G61" s="3" t="s">
         <v>465</v>
       </c>
-      <c r="G61" s="3" t="s">
+      <c r="H61" s="3" t="s">
         <v>466</v>
       </c>
-      <c r="H61" s="3" t="s">
+      <c r="I61" s="3" t="s">
         <v>467</v>
       </c>
-      <c r="I61" s="3" t="s">
+      <c r="J61" s="3" t="s">
         <v>468</v>
-      </c>
-      <c r="J61" s="3" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
@@ -5573,28 +5578,28 @@
         <v>48</v>
       </c>
       <c r="C62" t="s">
+        <v>469</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>470</v>
       </c>
-      <c r="D62" s="3" t="s">
+      <c r="E62" s="3" t="s">
         <v>471</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="F62" s="3" t="s">
         <v>472</v>
       </c>
-      <c r="F62" s="3" t="s">
+      <c r="G62" s="3" t="s">
         <v>473</v>
       </c>
-      <c r="G62" s="3" t="s">
+      <c r="H62" s="3" t="s">
         <v>474</v>
       </c>
-      <c r="H62" s="3" t="s">
+      <c r="I62" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="I62" s="3" t="s">
+      <c r="J62" s="3" t="s">
         <v>476</v>
-      </c>
-      <c r="J62" s="3" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
@@ -5605,28 +5610,28 @@
         <v>57</v>
       </c>
       <c r="C63" t="s">
+        <v>477</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="E63" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="F63" s="2" t="s">
         <v>480</v>
       </c>
-      <c r="F63" s="2" t="s">
+      <c r="G63" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="G63" s="2" t="s">
+      <c r="H63" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="H63" s="2" t="s">
+      <c r="I63" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="I63" s="2" t="s">
+      <c r="J63" s="2" t="s">
         <v>484</v>
-      </c>
-      <c r="J63" s="2" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -5637,7 +5642,7 @@
         <v>66</v>
       </c>
       <c r="C64" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D64" t="s">
         <v>71</v>
@@ -5655,10 +5660,10 @@
         <v>195</v>
       </c>
       <c r="I64" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J64" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
@@ -5672,57 +5677,57 @@
         <v>74</v>
       </c>
       <c r="D65" t="s">
+        <v>487</v>
+      </c>
+      <c r="E65" t="s">
         <v>488</v>
       </c>
-      <c r="E65" t="s">
+      <c r="F65" t="s">
         <v>489</v>
       </c>
-      <c r="F65" t="s">
+      <c r="G65" t="s">
         <v>490</v>
       </c>
-      <c r="G65" t="s">
+      <c r="H65" t="s">
         <v>491</v>
       </c>
-      <c r="H65" t="s">
+      <c r="I65" t="s">
         <v>492</v>
       </c>
-      <c r="I65" t="s">
+      <c r="J65" t="s">
         <v>493</v>
-      </c>
-      <c r="J65" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B66" t="s">
         <v>11</v>
       </c>
       <c r="C66" t="s">
+        <v>495</v>
+      </c>
+      <c r="D66" s="2" t="s">
         <v>496</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="E66" s="3" t="s">
         <v>497</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="F66" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="G66" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="G66" s="2" t="s">
+      <c r="H66" s="2" t="s">
         <v>500</v>
       </c>
-      <c r="H66" s="2" t="s">
+      <c r="I66" s="2" t="s">
         <v>501</v>
       </c>
-      <c r="I66" s="2" t="s">
+      <c r="J66" s="2" t="s">
         <v>502</v>
-      </c>
-      <c r="J66" s="2" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
@@ -5733,28 +5738,28 @@
         <v>21</v>
       </c>
       <c r="C67" t="s">
+        <v>503</v>
+      </c>
+      <c r="D67" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="D67" s="2" t="s">
+      <c r="E67" s="2" t="s">
         <v>505</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="F67" s="2" t="s">
         <v>506</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="G67" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="G67" s="2" t="s">
+      <c r="H67" s="2" t="s">
         <v>508</v>
       </c>
-      <c r="H67" s="2" t="s">
+      <c r="I67" s="2" t="s">
         <v>509</v>
       </c>
-      <c r="I67" s="2" t="s">
+      <c r="J67" s="2" t="s">
         <v>510</v>
-      </c>
-      <c r="J67" s="2" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
@@ -5765,28 +5770,28 @@
         <v>30</v>
       </c>
       <c r="C68" t="s">
+        <v>511</v>
+      </c>
+      <c r="D68" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="E68" s="3" t="s">
         <v>513</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="F68" s="3" t="s">
         <v>514</v>
       </c>
-      <c r="F68" s="3" t="s">
+      <c r="G68" s="3" t="s">
         <v>515</v>
       </c>
-      <c r="G68" s="3" t="s">
+      <c r="H68" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="H68" s="3" t="s">
+      <c r="I68" s="3" t="s">
         <v>517</v>
       </c>
-      <c r="I68" s="3" t="s">
+      <c r="J68" s="3" t="s">
         <v>518</v>
-      </c>
-      <c r="J68" s="3" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
@@ -5797,28 +5802,28 @@
         <v>39</v>
       </c>
       <c r="C69" t="s">
+        <v>519</v>
+      </c>
+      <c r="D69" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="E69" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="F69" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="G69" s="2" t="s">
         <v>523</v>
       </c>
-      <c r="G69" s="2" t="s">
+      <c r="H69" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="H69" s="2" t="s">
+      <c r="I69" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="I69" s="2" t="s">
+      <c r="J69" s="2" t="s">
         <v>526</v>
-      </c>
-      <c r="J69" s="2" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
@@ -5829,28 +5834,28 @@
         <v>48</v>
       </c>
       <c r="C70" t="s">
+        <v>527</v>
+      </c>
+      <c r="D70" s="2" t="s">
         <v>528</v>
       </c>
-      <c r="D70" s="2" t="s">
+      <c r="E70" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="E70" s="2" t="s">
+      <c r="F70" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="F70" s="2" t="s">
+      <c r="G70" s="3" t="s">
         <v>531</v>
       </c>
-      <c r="G70" s="3" t="s">
+      <c r="H70" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="H70" s="2" t="s">
+      <c r="I70" s="3" t="s">
         <v>533</v>
       </c>
-      <c r="I70" s="3" t="s">
+      <c r="J70" s="2" t="s">
         <v>534</v>
-      </c>
-      <c r="J70" s="2" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
@@ -5861,28 +5866,28 @@
         <v>57</v>
       </c>
       <c r="C71" t="s">
+        <v>535</v>
+      </c>
+      <c r="D71" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="E71" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="F71" s="2" t="s">
         <v>538</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="G71" s="2" t="s">
         <v>539</v>
       </c>
-      <c r="G71" s="2" t="s">
+      <c r="H71" s="2" t="s">
         <v>540</v>
       </c>
-      <c r="H71" s="2" t="s">
+      <c r="I71" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="I71" s="2" t="s">
+      <c r="J71" s="2" t="s">
         <v>542</v>
-      </c>
-      <c r="J71" s="2" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
@@ -5896,10 +5901,10 @@
         <v>67</v>
       </c>
       <c r="D72" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E72" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F72" t="s">
         <v>70</v>
@@ -5908,13 +5913,13 @@
         <v>69</v>
       </c>
       <c r="H72" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I72" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="J72" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
@@ -5928,57 +5933,57 @@
         <v>74</v>
       </c>
       <c r="D73" t="s">
+        <v>543</v>
+      </c>
+      <c r="E73" t="s">
         <v>544</v>
       </c>
-      <c r="E73" t="s">
+      <c r="F73" t="s">
         <v>545</v>
       </c>
-      <c r="F73" t="s">
+      <c r="G73" t="s">
+        <v>321</v>
+      </c>
+      <c r="H73" t="s">
         <v>546</v>
       </c>
-      <c r="G73" t="s">
-        <v>322</v>
-      </c>
-      <c r="H73" t="s">
+      <c r="I73" t="s">
         <v>547</v>
       </c>
-      <c r="I73" t="s">
+      <c r="J73" t="s">
         <v>548</v>
-      </c>
-      <c r="J73" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>550</v>
+        <v>1062</v>
       </c>
       <c r="B74" t="s">
         <v>11</v>
       </c>
       <c r="C74" t="s">
+        <v>549</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="E74" s="2" t="s">
         <v>551</v>
       </c>
-      <c r="D74" s="2" t="s">
+      <c r="F74" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="G74" s="2" t="s">
         <v>553</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="H74" s="2" t="s">
         <v>554</v>
       </c>
-      <c r="G74" s="2" t="s">
+      <c r="I74" s="2" t="s">
         <v>555</v>
       </c>
-      <c r="H74" s="2" t="s">
+      <c r="J74" s="2" t="s">
         <v>556</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>557</v>
-      </c>
-      <c r="J74" s="2" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
@@ -5989,28 +5994,28 @@
         <v>21</v>
       </c>
       <c r="C75" t="s">
+        <v>557</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>558</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>559</v>
       </c>
-      <c r="D75" s="2" t="s">
+      <c r="F75" s="2" t="s">
         <v>560</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="G75" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="H75" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="G75" s="2" t="s">
+      <c r="I75" s="2" t="s">
         <v>563</v>
       </c>
-      <c r="H75" s="2" t="s">
+      <c r="J75" s="2" t="s">
         <v>564</v>
-      </c>
-      <c r="I75" s="2" t="s">
-        <v>565</v>
-      </c>
-      <c r="J75" s="2" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
@@ -6021,28 +6026,28 @@
         <v>30</v>
       </c>
       <c r="C76" t="s">
+        <v>565</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="E76" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="F76" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="G76" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="F76" s="2" t="s">
+      <c r="H76" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="G76" s="2" t="s">
+      <c r="I76" s="2" t="s">
         <v>571</v>
       </c>
-      <c r="H76" s="2" t="s">
+      <c r="J76" s="2" t="s">
         <v>572</v>
-      </c>
-      <c r="I76" s="2" t="s">
-        <v>573</v>
-      </c>
-      <c r="J76" s="2" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
@@ -6053,28 +6058,28 @@
         <v>39</v>
       </c>
       <c r="C77" t="s">
+        <v>573</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="E77" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="F77" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="E77" s="2" t="s">
+      <c r="G77" s="2" t="s">
         <v>577</v>
       </c>
-      <c r="F77" s="2" t="s">
+      <c r="H77" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="G77" s="2" t="s">
+      <c r="I77" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="H77" s="2" t="s">
+      <c r="J77" s="2" t="s">
         <v>580</v>
-      </c>
-      <c r="I77" s="2" t="s">
-        <v>581</v>
-      </c>
-      <c r="J77" s="2" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
@@ -6085,28 +6090,28 @@
         <v>48</v>
       </c>
       <c r="C78" t="s">
+        <v>581</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="E78" s="2" t="s">
         <v>583</v>
       </c>
-      <c r="D78" s="2" t="s">
+      <c r="F78" s="2" t="s">
         <v>584</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="G78" s="2" t="s">
         <v>585</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="H78" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="G78" s="2" t="s">
+      <c r="I78" s="2" t="s">
         <v>587</v>
       </c>
-      <c r="H78" s="2" t="s">
+      <c r="J78" s="2" t="s">
         <v>588</v>
-      </c>
-      <c r="I78" s="2" t="s">
-        <v>589</v>
-      </c>
-      <c r="J78" s="2" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
@@ -6117,28 +6122,28 @@
         <v>57</v>
       </c>
       <c r="C79" t="s">
+        <v>589</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="E79" s="2" t="s">
         <v>591</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="F79" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="G79" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="H79" s="2" t="s">
         <v>594</v>
       </c>
-      <c r="G79" s="2" t="s">
+      <c r="I79" s="2" t="s">
         <v>595</v>
       </c>
-      <c r="H79" s="2" t="s">
+      <c r="J79" s="2" t="s">
         <v>596</v>
-      </c>
-      <c r="I79" s="2" t="s">
-        <v>597</v>
-      </c>
-      <c r="J79" s="2" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
@@ -6149,7 +6154,7 @@
         <v>66</v>
       </c>
       <c r="C80" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="D80" t="s">
         <v>67</v>
@@ -6167,7 +6172,7 @@
         <v>195</v>
       </c>
       <c r="I80" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="J80" t="s">
         <v>136</v>
@@ -6184,57 +6189,57 @@
         <v>74</v>
       </c>
       <c r="D81" t="s">
+        <v>599</v>
+      </c>
+      <c r="E81" t="s">
+        <v>600</v>
+      </c>
+      <c r="F81" t="s">
         <v>601</v>
       </c>
-      <c r="E81" t="s">
+      <c r="G81" t="s">
         <v>602</v>
       </c>
-      <c r="F81" t="s">
+      <c r="H81" t="s">
         <v>603</v>
       </c>
-      <c r="G81" t="s">
+      <c r="I81" t="s">
         <v>604</v>
       </c>
-      <c r="H81" t="s">
+      <c r="J81" t="s">
         <v>605</v>
-      </c>
-      <c r="I81" t="s">
-        <v>606</v>
-      </c>
-      <c r="J81" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="B82" t="s">
         <v>11</v>
       </c>
       <c r="C82" t="s">
+        <v>607</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="E82" s="3" t="s">
         <v>609</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="F82" s="2" t="s">
         <v>610</v>
       </c>
-      <c r="E82" s="3" t="s">
+      <c r="G82" s="2" t="s">
         <v>611</v>
       </c>
-      <c r="F82" s="2" t="s">
+      <c r="H82" s="3" t="s">
         <v>612</v>
       </c>
-      <c r="G82" s="2" t="s">
+      <c r="I82" s="2" t="s">
         <v>613</v>
       </c>
-      <c r="H82" s="3" t="s">
+      <c r="J82" s="3" t="s">
         <v>614</v>
-      </c>
-      <c r="I82" s="2" t="s">
-        <v>615</v>
-      </c>
-      <c r="J82" s="3" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
@@ -6245,28 +6250,28 @@
         <v>21</v>
       </c>
       <c r="C83" t="s">
+        <v>615</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="E83" s="2" t="s">
         <v>617</v>
       </c>
-      <c r="D83" s="2" t="s">
+      <c r="F83" s="2" t="s">
         <v>618</v>
       </c>
-      <c r="E83" s="2" t="s">
+      <c r="G83" s="2" t="s">
         <v>619</v>
       </c>
-      <c r="F83" s="2" t="s">
+      <c r="H83" s="2" t="s">
         <v>620</v>
       </c>
-      <c r="G83" s="2" t="s">
+      <c r="I83" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="H83" s="2" t="s">
+      <c r="J83" s="2" t="s">
         <v>622</v>
-      </c>
-      <c r="I83" s="2" t="s">
-        <v>623</v>
-      </c>
-      <c r="J83" s="2" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
@@ -6277,28 +6282,28 @@
         <v>30</v>
       </c>
       <c r="C84" t="s">
+        <v>623</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>624</v>
+      </c>
+      <c r="E84" s="3" t="s">
         <v>625</v>
       </c>
-      <c r="D84" s="3" t="s">
+      <c r="F84" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="E84" s="3" t="s">
+      <c r="G84" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="F84" s="3" t="s">
+      <c r="H84" s="2" t="s">
         <v>628</v>
       </c>
-      <c r="G84" s="2" t="s">
+      <c r="I84" s="2" t="s">
         <v>629</v>
       </c>
-      <c r="H84" s="2" t="s">
+      <c r="J84" s="2" t="s">
         <v>630</v>
-      </c>
-      <c r="I84" s="2" t="s">
-        <v>631</v>
-      </c>
-      <c r="J84" s="2" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
@@ -6309,28 +6314,28 @@
         <v>39</v>
       </c>
       <c r="C85" t="s">
+        <v>631</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="E85" s="2" t="s">
         <v>633</v>
       </c>
-      <c r="D85" s="2" t="s">
+      <c r="F85" s="3" t="s">
         <v>634</v>
       </c>
-      <c r="E85" s="2" t="s">
+      <c r="G85" s="2" t="s">
         <v>635</v>
       </c>
-      <c r="F85" s="3" t="s">
+      <c r="H85" s="2" t="s">
         <v>636</v>
       </c>
-      <c r="G85" s="2" t="s">
+      <c r="I85" s="2" t="s">
         <v>637</v>
       </c>
-      <c r="H85" s="2" t="s">
+      <c r="J85" s="2" t="s">
         <v>638</v>
-      </c>
-      <c r="I85" s="2" t="s">
-        <v>639</v>
-      </c>
-      <c r="J85" s="2" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
@@ -6341,28 +6346,28 @@
         <v>48</v>
       </c>
       <c r="C86" t="s">
+        <v>639</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="E86" s="2" t="s">
         <v>641</v>
       </c>
-      <c r="D86" s="2" t="s">
+      <c r="F86" s="2" t="s">
         <v>642</v>
       </c>
-      <c r="E86" s="2" t="s">
+      <c r="G86" s="2" t="s">
         <v>643</v>
       </c>
-      <c r="F86" s="2" t="s">
+      <c r="H86" s="2" t="s">
         <v>644</v>
       </c>
-      <c r="G86" s="2" t="s">
+      <c r="I86" s="2" t="s">
         <v>645</v>
       </c>
-      <c r="H86" s="2" t="s">
+      <c r="J86" s="2" t="s">
         <v>646</v>
-      </c>
-      <c r="I86" s="2" t="s">
-        <v>647</v>
-      </c>
-      <c r="J86" s="2" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
@@ -6373,28 +6378,28 @@
         <v>57</v>
       </c>
       <c r="C87" t="s">
+        <v>647</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="E87" s="2" t="s">
         <v>649</v>
       </c>
-      <c r="D87" s="2" t="s">
+      <c r="F87" s="2" t="s">
         <v>650</v>
       </c>
-      <c r="E87" s="2" t="s">
+      <c r="G87" s="2" t="s">
         <v>651</v>
       </c>
-      <c r="F87" s="2" t="s">
+      <c r="H87" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="G87" s="2" t="s">
+      <c r="I87" s="2" t="s">
         <v>653</v>
       </c>
-      <c r="H87" s="2" t="s">
+      <c r="J87" s="2" t="s">
         <v>654</v>
-      </c>
-      <c r="I87" s="2" t="s">
-        <v>655</v>
-      </c>
-      <c r="J87" s="2" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
@@ -6405,7 +6410,7 @@
         <v>66</v>
       </c>
       <c r="C88" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D88" t="s">
         <v>195</v>
@@ -6414,10 +6419,10 @@
         <v>193</v>
       </c>
       <c r="F88" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G88" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H88" t="s">
         <v>72</v>
@@ -6440,57 +6445,57 @@
         <v>74</v>
       </c>
       <c r="D89" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E89" t="s">
+        <v>655</v>
+      </c>
+      <c r="F89" t="s">
+        <v>656</v>
+      </c>
+      <c r="G89" t="s">
         <v>657</v>
       </c>
-      <c r="F89" t="s">
+      <c r="H89" t="s">
         <v>658</v>
       </c>
-      <c r="G89" t="s">
+      <c r="I89" t="s">
+        <v>543</v>
+      </c>
+      <c r="J89" t="s">
         <v>659</v>
-      </c>
-      <c r="H89" t="s">
-        <v>660</v>
-      </c>
-      <c r="I89" t="s">
-        <v>544</v>
-      </c>
-      <c r="J89" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="B90" t="s">
         <v>11</v>
       </c>
       <c r="C90" t="s">
+        <v>661</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="E90" s="2" t="s">
         <v>663</v>
       </c>
-      <c r="D90" s="2" t="s">
+      <c r="F90" s="2" t="s">
         <v>664</v>
       </c>
-      <c r="E90" s="2" t="s">
+      <c r="G90" s="2" t="s">
         <v>665</v>
       </c>
-      <c r="F90" s="2" t="s">
+      <c r="H90" s="2" t="s">
         <v>666</v>
       </c>
-      <c r="G90" s="2" t="s">
+      <c r="I90" s="2" t="s">
         <v>667</v>
       </c>
-      <c r="H90" s="2" t="s">
+      <c r="J90" s="2" t="s">
         <v>668</v>
-      </c>
-      <c r="I90" s="2" t="s">
-        <v>669</v>
-      </c>
-      <c r="J90" s="2" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
@@ -6501,28 +6506,28 @@
         <v>21</v>
       </c>
       <c r="C91" t="s">
+        <v>669</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>670</v>
+      </c>
+      <c r="E91" s="2" t="s">
         <v>671</v>
       </c>
-      <c r="D91" s="3" t="s">
+      <c r="F91" t="s">
         <v>672</v>
       </c>
-      <c r="E91" s="2" t="s">
+      <c r="G91" s="2" t="s">
         <v>673</v>
       </c>
-      <c r="F91" t="s">
+      <c r="H91" s="2" t="s">
         <v>674</v>
       </c>
-      <c r="G91" s="2" t="s">
+      <c r="I91" s="2" t="s">
         <v>675</v>
       </c>
-      <c r="H91" s="2" t="s">
+      <c r="J91" s="2" t="s">
         <v>676</v>
-      </c>
-      <c r="I91" s="2" t="s">
-        <v>677</v>
-      </c>
-      <c r="J91" s="2" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
@@ -6533,28 +6538,28 @@
         <v>30</v>
       </c>
       <c r="C92" t="s">
+        <v>677</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="E92" s="2" t="s">
         <v>679</v>
       </c>
-      <c r="D92" s="2" t="s">
+      <c r="F92" s="2" t="s">
         <v>680</v>
       </c>
-      <c r="E92" s="2" t="s">
+      <c r="G92" s="2" t="s">
         <v>681</v>
       </c>
-      <c r="F92" s="2" t="s">
+      <c r="H92" s="2" t="s">
         <v>682</v>
       </c>
-      <c r="G92" s="2" t="s">
+      <c r="I92" s="2" t="s">
         <v>683</v>
       </c>
-      <c r="H92" s="2" t="s">
+      <c r="J92" s="2" t="s">
         <v>684</v>
-      </c>
-      <c r="I92" s="2" t="s">
-        <v>685</v>
-      </c>
-      <c r="J92" s="2" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
@@ -6565,28 +6570,28 @@
         <v>39</v>
       </c>
       <c r="C93" t="s">
+        <v>685</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="E93" s="2" t="s">
         <v>687</v>
       </c>
-      <c r="D93" s="2" t="s">
+      <c r="F93" s="2" t="s">
         <v>688</v>
       </c>
-      <c r="E93" s="2" t="s">
+      <c r="G93" s="3" t="s">
         <v>689</v>
       </c>
-      <c r="F93" s="2" t="s">
+      <c r="H93" s="3" t="s">
         <v>690</v>
       </c>
-      <c r="G93" s="3" t="s">
+      <c r="I93" s="3" t="s">
         <v>691</v>
       </c>
-      <c r="H93" s="3" t="s">
+      <c r="J93" s="3" t="s">
         <v>692</v>
-      </c>
-      <c r="I93" s="3" t="s">
-        <v>693</v>
-      </c>
-      <c r="J93" s="3" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
@@ -6597,28 +6602,28 @@
         <v>48</v>
       </c>
       <c r="C94" t="s">
+        <v>693</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="E94" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="D94" s="2" t="s">
+      <c r="F94" s="2" t="s">
         <v>696</v>
       </c>
-      <c r="E94" s="2" t="s">
+      <c r="G94" s="2" t="s">
         <v>697</v>
       </c>
-      <c r="F94" s="2" t="s">
+      <c r="H94" s="2" t="s">
         <v>698</v>
       </c>
-      <c r="G94" s="2" t="s">
+      <c r="I94" s="2" t="s">
         <v>699</v>
       </c>
-      <c r="H94" s="2" t="s">
+      <c r="J94" s="2" t="s">
         <v>700</v>
-      </c>
-      <c r="I94" s="2" t="s">
-        <v>701</v>
-      </c>
-      <c r="J94" s="2" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
@@ -6629,28 +6634,28 @@
         <v>57</v>
       </c>
       <c r="C95" t="s">
+        <v>701</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="E95" s="2" t="s">
         <v>703</v>
       </c>
-      <c r="D95" s="2" t="s">
+      <c r="F95" s="2" t="s">
         <v>704</v>
       </c>
-      <c r="E95" s="2" t="s">
+      <c r="G95" s="2" t="s">
         <v>705</v>
       </c>
-      <c r="F95" s="2" t="s">
+      <c r="H95" s="2" t="s">
         <v>706</v>
       </c>
-      <c r="G95" s="2" t="s">
+      <c r="I95" s="2" t="s">
         <v>707</v>
       </c>
-      <c r="H95" s="2" t="s">
+      <c r="J95" s="2" t="s">
         <v>708</v>
-      </c>
-      <c r="I95" s="2" t="s">
-        <v>709</v>
-      </c>
-      <c r="J95" s="2" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
@@ -6664,13 +6669,13 @@
         <v>253</v>
       </c>
       <c r="D96" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E96" t="s">
         <v>69</v>
       </c>
       <c r="F96" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G96" t="s">
         <v>255</v>
@@ -6696,57 +6701,57 @@
         <v>74</v>
       </c>
       <c r="D97" t="s">
+        <v>709</v>
+      </c>
+      <c r="E97" t="s">
+        <v>710</v>
+      </c>
+      <c r="F97" t="s">
         <v>711</v>
       </c>
-      <c r="E97" t="s">
+      <c r="G97" t="s">
         <v>712</v>
       </c>
-      <c r="F97" t="s">
+      <c r="H97" t="s">
         <v>713</v>
       </c>
-      <c r="G97" t="s">
+      <c r="I97" t="s">
         <v>714</v>
       </c>
-      <c r="H97" t="s">
+      <c r="J97" t="s">
         <v>715</v>
-      </c>
-      <c r="I97" t="s">
-        <v>716</v>
-      </c>
-      <c r="J97" t="s">
-        <v>717</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B98" t="s">
         <v>11</v>
       </c>
       <c r="C98" t="s">
+        <v>717</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="E98" s="2" t="s">
         <v>719</v>
       </c>
-      <c r="D98" s="2" t="s">
+      <c r="F98" s="2" t="s">
         <v>720</v>
       </c>
-      <c r="E98" s="2" t="s">
+      <c r="G98" s="2" t="s">
         <v>721</v>
       </c>
-      <c r="F98" s="2" t="s">
+      <c r="H98" s="2" t="s">
         <v>722</v>
       </c>
-      <c r="G98" s="2" t="s">
+      <c r="I98" s="2" t="s">
         <v>723</v>
       </c>
-      <c r="H98" s="2" t="s">
+      <c r="J98" s="2" t="s">
         <v>724</v>
-      </c>
-      <c r="I98" s="2" t="s">
-        <v>725</v>
-      </c>
-      <c r="J98" s="2" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
@@ -6757,28 +6762,28 @@
         <v>21</v>
       </c>
       <c r="C99" t="s">
+        <v>725</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>726</v>
+      </c>
+      <c r="E99" s="3" t="s">
         <v>727</v>
       </c>
-      <c r="D99" s="3" t="s">
+      <c r="F99" s="3" t="s">
         <v>728</v>
       </c>
-      <c r="E99" s="3" t="s">
+      <c r="G99" s="3" t="s">
         <v>729</v>
       </c>
-      <c r="F99" s="3" t="s">
+      <c r="H99" s="3" t="s">
         <v>730</v>
       </c>
-      <c r="G99" s="3" t="s">
+      <c r="I99" s="3" t="s">
         <v>731</v>
       </c>
-      <c r="H99" s="3" t="s">
+      <c r="J99" s="3" t="s">
         <v>732</v>
-      </c>
-      <c r="I99" s="3" t="s">
-        <v>733</v>
-      </c>
-      <c r="J99" s="3" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
@@ -6789,28 +6794,28 @@
         <v>30</v>
       </c>
       <c r="C100" t="s">
+        <v>733</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="E100" s="3" t="s">
         <v>735</v>
       </c>
-      <c r="D100" s="3" t="s">
+      <c r="F100" s="3" t="s">
         <v>736</v>
       </c>
-      <c r="E100" s="3" t="s">
+      <c r="G100" s="3" t="s">
         <v>737</v>
       </c>
-      <c r="F100" s="3" t="s">
+      <c r="H100" s="3" t="s">
         <v>738</v>
       </c>
-      <c r="G100" s="3" t="s">
+      <c r="I100" s="3" t="s">
         <v>739</v>
       </c>
-      <c r="H100" s="3" t="s">
+      <c r="J100" s="3" t="s">
         <v>740</v>
-      </c>
-      <c r="I100" s="3" t="s">
-        <v>741</v>
-      </c>
-      <c r="J100" s="3" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
@@ -6821,28 +6826,28 @@
         <v>39</v>
       </c>
       <c r="C101" t="s">
+        <v>741</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="E101" s="3" t="s">
         <v>743</v>
       </c>
-      <c r="D101" s="2" t="s">
+      <c r="F101" s="3" t="s">
         <v>744</v>
       </c>
-      <c r="E101" s="3" t="s">
+      <c r="G101" s="3" t="s">
         <v>745</v>
       </c>
-      <c r="F101" s="3" t="s">
+      <c r="H101" s="3" t="s">
         <v>746</v>
       </c>
-      <c r="G101" s="3" t="s">
+      <c r="I101" s="3" t="s">
         <v>747</v>
       </c>
-      <c r="H101" s="3" t="s">
+      <c r="J101" s="3" t="s">
         <v>748</v>
-      </c>
-      <c r="I101" s="3" t="s">
-        <v>749</v>
-      </c>
-      <c r="J101" s="3" t="s">
-        <v>750</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
@@ -6853,28 +6858,28 @@
         <v>48</v>
       </c>
       <c r="C102" t="s">
+        <v>749</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="E102" s="2" t="s">
         <v>751</v>
       </c>
-      <c r="D102" s="2" t="s">
+      <c r="F102" s="2" t="s">
         <v>752</v>
       </c>
-      <c r="E102" s="2" t="s">
+      <c r="G102" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="F102" s="2" t="s">
+      <c r="H102" s="2" t="s">
         <v>754</v>
       </c>
-      <c r="G102" s="2" t="s">
+      <c r="I102" s="2" t="s">
         <v>755</v>
       </c>
-      <c r="H102" s="2" t="s">
+      <c r="J102" s="2" t="s">
         <v>756</v>
-      </c>
-      <c r="I102" s="2" t="s">
-        <v>757</v>
-      </c>
-      <c r="J102" s="2" t="s">
-        <v>758</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
@@ -6885,28 +6890,28 @@
         <v>57</v>
       </c>
       <c r="C103" t="s">
+        <v>757</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="E103" s="2" t="s">
         <v>759</v>
       </c>
-      <c r="D103" s="3" t="s">
+      <c r="F103" s="2" t="s">
         <v>760</v>
       </c>
-      <c r="E103" s="2" t="s">
+      <c r="G103" s="3" t="s">
         <v>761</v>
       </c>
-      <c r="F103" s="2" t="s">
+      <c r="H103" s="3" t="s">
         <v>762</v>
       </c>
-      <c r="G103" s="3" t="s">
+      <c r="I103" s="2" t="s">
         <v>763</v>
       </c>
-      <c r="H103" s="3" t="s">
+      <c r="J103" s="3" t="s">
         <v>764</v>
-      </c>
-      <c r="I103" s="2" t="s">
-        <v>765</v>
-      </c>
-      <c r="J103" s="3" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
@@ -6920,19 +6925,19 @@
         <v>195</v>
       </c>
       <c r="D104" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E104" t="s">
         <v>72</v>
       </c>
       <c r="F104" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G104" t="s">
         <v>195</v>
       </c>
       <c r="H104" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="I104" t="s">
         <v>72</v>
@@ -6952,57 +6957,57 @@
         <v>74</v>
       </c>
       <c r="D105" t="s">
+        <v>765</v>
+      </c>
+      <c r="E105" t="s">
+        <v>766</v>
+      </c>
+      <c r="F105" t="s">
         <v>767</v>
       </c>
-      <c r="E105" t="s">
+      <c r="G105" t="s">
         <v>768</v>
       </c>
-      <c r="F105" t="s">
+      <c r="H105" t="s">
         <v>769</v>
       </c>
-      <c r="G105" t="s">
+      <c r="I105" t="s">
         <v>770</v>
       </c>
-      <c r="H105" t="s">
+      <c r="J105" t="s">
         <v>771</v>
-      </c>
-      <c r="I105" t="s">
-        <v>772</v>
-      </c>
-      <c r="J105" t="s">
-        <v>773</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="B106" t="s">
         <v>11</v>
       </c>
       <c r="C106" t="s">
+        <v>773</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>774</v>
+      </c>
+      <c r="E106" s="3" t="s">
         <v>775</v>
       </c>
-      <c r="D106" s="3" t="s">
+      <c r="F106" s="3" t="s">
         <v>776</v>
       </c>
-      <c r="E106" s="3" t="s">
+      <c r="G106" s="3" t="s">
         <v>777</v>
       </c>
-      <c r="F106" s="3" t="s">
+      <c r="H106" s="3" t="s">
         <v>778</v>
       </c>
-      <c r="G106" s="3" t="s">
+      <c r="I106" s="3" t="s">
         <v>779</v>
       </c>
-      <c r="H106" s="3" t="s">
+      <c r="J106" s="3" t="s">
         <v>780</v>
-      </c>
-      <c r="I106" s="3" t="s">
-        <v>781</v>
-      </c>
-      <c r="J106" s="3" t="s">
-        <v>782</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
@@ -7013,28 +7018,28 @@
         <v>21</v>
       </c>
       <c r="C107" t="s">
+        <v>781</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>782</v>
+      </c>
+      <c r="E107" s="3" t="s">
         <v>783</v>
       </c>
-      <c r="D107" s="3" t="s">
+      <c r="F107" s="3" t="s">
         <v>784</v>
       </c>
-      <c r="E107" s="3" t="s">
+      <c r="G107" s="3" t="s">
         <v>785</v>
       </c>
-      <c r="F107" s="3" t="s">
+      <c r="H107" s="3" t="s">
         <v>786</v>
       </c>
-      <c r="G107" s="3" t="s">
+      <c r="I107" s="3" t="s">
         <v>787</v>
       </c>
-      <c r="H107" s="3" t="s">
+      <c r="J107" s="3" t="s">
         <v>788</v>
-      </c>
-      <c r="I107" s="3" t="s">
-        <v>789</v>
-      </c>
-      <c r="J107" s="3" t="s">
-        <v>790</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
@@ -7045,28 +7050,28 @@
         <v>30</v>
       </c>
       <c r="C108" t="s">
+        <v>789</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="E108" s="2" t="s">
         <v>791</v>
       </c>
-      <c r="D108" s="3" t="s">
+      <c r="F108" s="2" t="s">
         <v>792</v>
       </c>
-      <c r="E108" s="2" t="s">
+      <c r="G108" s="2" t="s">
         <v>793</v>
       </c>
-      <c r="F108" s="2" t="s">
+      <c r="H108" s="2" t="s">
         <v>794</v>
       </c>
-      <c r="G108" s="2" t="s">
+      <c r="I108" s="2" t="s">
         <v>795</v>
       </c>
-      <c r="H108" s="2" t="s">
+      <c r="J108" s="2" t="s">
         <v>796</v>
-      </c>
-      <c r="I108" s="2" t="s">
-        <v>797</v>
-      </c>
-      <c r="J108" s="2" t="s">
-        <v>798</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
@@ -7077,28 +7082,28 @@
         <v>39</v>
       </c>
       <c r="C109" t="s">
+        <v>797</v>
+      </c>
+      <c r="D109" t="s">
+        <v>798</v>
+      </c>
+      <c r="E109" s="3" t="s">
         <v>799</v>
       </c>
-      <c r="D109" t="s">
+      <c r="F109" s="3" t="s">
         <v>800</v>
       </c>
-      <c r="E109" s="3" t="s">
+      <c r="G109" s="3" t="s">
         <v>801</v>
       </c>
-      <c r="F109" s="3" t="s">
+      <c r="H109" s="3" t="s">
         <v>802</v>
       </c>
-      <c r="G109" s="3" t="s">
+      <c r="I109" s="3" t="s">
         <v>803</v>
       </c>
-      <c r="H109" s="3" t="s">
+      <c r="J109" s="3" t="s">
         <v>804</v>
-      </c>
-      <c r="I109" s="3" t="s">
-        <v>805</v>
-      </c>
-      <c r="J109" s="3" t="s">
-        <v>806</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
@@ -7109,28 +7114,28 @@
         <v>48</v>
       </c>
       <c r="C110" t="s">
+        <v>805</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>806</v>
+      </c>
+      <c r="E110" s="2" t="s">
         <v>807</v>
       </c>
-      <c r="D110" s="3" t="s">
+      <c r="F110" s="2" t="s">
         <v>808</v>
       </c>
-      <c r="E110" s="2" t="s">
+      <c r="G110" s="2" t="s">
         <v>809</v>
       </c>
-      <c r="F110" s="2" t="s">
+      <c r="H110" s="2" t="s">
         <v>810</v>
       </c>
-      <c r="G110" s="2" t="s">
+      <c r="I110" s="2" t="s">
         <v>811</v>
       </c>
-      <c r="H110" s="2" t="s">
+      <c r="J110" s="2" t="s">
         <v>812</v>
-      </c>
-      <c r="I110" s="2" t="s">
-        <v>813</v>
-      </c>
-      <c r="J110" s="2" t="s">
-        <v>814</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
@@ -7141,28 +7146,28 @@
         <v>57</v>
       </c>
       <c r="C111" t="s">
+        <v>813</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>814</v>
+      </c>
+      <c r="E111" s="2" t="s">
         <v>815</v>
       </c>
-      <c r="D111" s="2" t="s">
+      <c r="F111" s="2" t="s">
         <v>816</v>
       </c>
-      <c r="E111" s="2" t="s">
+      <c r="G111" s="2" t="s">
         <v>817</v>
       </c>
-      <c r="F111" s="2" t="s">
+      <c r="H111" s="2" t="s">
         <v>818</v>
       </c>
-      <c r="G111" s="2" t="s">
+      <c r="I111" s="2" t="s">
         <v>819</v>
       </c>
-      <c r="H111" s="2" t="s">
+      <c r="J111" s="2" t="s">
         <v>820</v>
-      </c>
-      <c r="I111" s="2" t="s">
-        <v>821</v>
-      </c>
-      <c r="J111" s="2" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
@@ -7176,7 +7181,7 @@
         <v>72</v>
       </c>
       <c r="D112" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="E112" t="s">
         <v>196</v>
@@ -7188,7 +7193,7 @@
         <v>195</v>
       </c>
       <c r="H112" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I112" t="s">
         <v>136</v>
@@ -7208,57 +7213,57 @@
         <v>74</v>
       </c>
       <c r="D113" t="s">
+        <v>822</v>
+      </c>
+      <c r="E113" t="s">
+        <v>823</v>
+      </c>
+      <c r="F113" t="s">
         <v>824</v>
       </c>
-      <c r="E113" t="s">
+      <c r="G113" t="s">
         <v>825</v>
       </c>
-      <c r="F113" t="s">
+      <c r="H113" t="s">
         <v>826</v>
       </c>
-      <c r="G113" t="s">
+      <c r="I113" t="s">
         <v>827</v>
       </c>
-      <c r="H113" t="s">
+      <c r="J113" t="s">
         <v>828</v>
-      </c>
-      <c r="I113" t="s">
-        <v>829</v>
-      </c>
-      <c r="J113" t="s">
-        <v>830</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="B114" t="s">
         <v>11</v>
       </c>
       <c r="C114" t="s">
+        <v>830</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>831</v>
+      </c>
+      <c r="E114" s="3" t="s">
         <v>832</v>
       </c>
-      <c r="D114" s="3" t="s">
+      <c r="F114" s="3" t="s">
         <v>833</v>
       </c>
-      <c r="E114" s="3" t="s">
+      <c r="G114" s="3" t="s">
         <v>834</v>
       </c>
-      <c r="F114" s="3" t="s">
+      <c r="H114" s="3" t="s">
         <v>835</v>
       </c>
-      <c r="G114" s="3" t="s">
+      <c r="I114" s="3" t="s">
         <v>836</v>
       </c>
-      <c r="H114" s="3" t="s">
+      <c r="J114" s="3" t="s">
         <v>837</v>
-      </c>
-      <c r="I114" s="3" t="s">
-        <v>838</v>
-      </c>
-      <c r="J114" s="3" t="s">
-        <v>839</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
@@ -7269,28 +7274,28 @@
         <v>21</v>
       </c>
       <c r="C115" t="s">
+        <v>838</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>839</v>
+      </c>
+      <c r="E115" s="3" t="s">
         <v>840</v>
       </c>
-      <c r="D115" s="3" t="s">
+      <c r="F115" s="3" t="s">
         <v>841</v>
       </c>
-      <c r="E115" s="3" t="s">
+      <c r="G115" s="3" t="s">
         <v>842</v>
       </c>
-      <c r="F115" s="3" t="s">
+      <c r="H115" s="3" t="s">
         <v>843</v>
       </c>
-      <c r="G115" s="3" t="s">
+      <c r="I115" s="3" t="s">
         <v>844</v>
       </c>
-      <c r="H115" s="3" t="s">
+      <c r="J115" s="3" t="s">
         <v>845</v>
-      </c>
-      <c r="I115" s="3" t="s">
-        <v>846</v>
-      </c>
-      <c r="J115" s="3" t="s">
-        <v>847</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
@@ -7301,28 +7306,28 @@
         <v>30</v>
       </c>
       <c r="C116" t="s">
+        <v>846</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>847</v>
+      </c>
+      <c r="E116" s="3" t="s">
         <v>848</v>
       </c>
-      <c r="D116" s="3" t="s">
+      <c r="F116" s="3" t="s">
         <v>849</v>
       </c>
-      <c r="E116" s="3" t="s">
+      <c r="G116" s="3" t="s">
         <v>850</v>
       </c>
-      <c r="F116" s="3" t="s">
+      <c r="H116" s="3" t="s">
         <v>851</v>
       </c>
-      <c r="G116" s="3" t="s">
+      <c r="I116" s="3" t="s">
         <v>852</v>
       </c>
-      <c r="H116" s="3" t="s">
+      <c r="J116" s="3" t="s">
         <v>853</v>
-      </c>
-      <c r="I116" s="3" t="s">
-        <v>854</v>
-      </c>
-      <c r="J116" s="3" t="s">
-        <v>855</v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.25">
@@ -7333,28 +7338,28 @@
         <v>39</v>
       </c>
       <c r="C117" t="s">
+        <v>854</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>855</v>
+      </c>
+      <c r="E117" s="2" t="s">
         <v>856</v>
       </c>
-      <c r="D117" s="2" t="s">
+      <c r="F117" s="2" t="s">
         <v>857</v>
       </c>
-      <c r="E117" s="2" t="s">
+      <c r="G117" s="2" t="s">
         <v>858</v>
       </c>
-      <c r="F117" s="2" t="s">
+      <c r="H117" s="2" t="s">
         <v>859</v>
       </c>
-      <c r="G117" s="2" t="s">
+      <c r="I117" s="2" t="s">
         <v>860</v>
       </c>
-      <c r="H117" s="2" t="s">
+      <c r="J117" s="2" t="s">
         <v>861</v>
-      </c>
-      <c r="I117" s="2" t="s">
-        <v>862</v>
-      </c>
-      <c r="J117" s="2" t="s">
-        <v>863</v>
       </c>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.25">
@@ -7365,28 +7370,28 @@
         <v>48</v>
       </c>
       <c r="C118" t="s">
+        <v>862</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>863</v>
+      </c>
+      <c r="E118" s="3" t="s">
         <v>864</v>
       </c>
-      <c r="D118" s="2" t="s">
+      <c r="F118" s="3" t="s">
         <v>865</v>
       </c>
-      <c r="E118" s="3" t="s">
+      <c r="G118" s="2" t="s">
         <v>866</v>
       </c>
-      <c r="F118" s="3" t="s">
+      <c r="H118" s="2" t="s">
         <v>867</v>
       </c>
-      <c r="G118" s="2" t="s">
+      <c r="I118" s="2" t="s">
         <v>868</v>
       </c>
-      <c r="H118" s="2" t="s">
+      <c r="J118" s="2" t="s">
         <v>869</v>
-      </c>
-      <c r="I118" s="2" t="s">
-        <v>870</v>
-      </c>
-      <c r="J118" s="2" t="s">
-        <v>871</v>
       </c>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.25">
@@ -7397,28 +7402,28 @@
         <v>57</v>
       </c>
       <c r="C119" t="s">
+        <v>870</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>871</v>
+      </c>
+      <c r="E119" s="2" t="s">
         <v>872</v>
       </c>
-      <c r="D119" s="2" t="s">
+      <c r="F119" s="2" t="s">
         <v>873</v>
       </c>
-      <c r="E119" s="2" t="s">
+      <c r="G119" s="2" t="s">
         <v>874</v>
       </c>
-      <c r="F119" s="2" t="s">
+      <c r="H119" s="2" t="s">
         <v>875</v>
       </c>
-      <c r="G119" s="2" t="s">
+      <c r="I119" s="2" t="s">
         <v>876</v>
       </c>
-      <c r="H119" s="2" t="s">
+      <c r="J119" s="2" t="s">
         <v>877</v>
-      </c>
-      <c r="I119" s="2" t="s">
-        <v>878</v>
-      </c>
-      <c r="J119" s="2" t="s">
-        <v>879</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.25">
@@ -7435,10 +7440,10 @@
         <v>195</v>
       </c>
       <c r="E120" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="F120" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G120" t="s">
         <v>256</v>
@@ -7447,10 +7452,10 @@
         <v>194</v>
       </c>
       <c r="I120" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="J120" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.25">
@@ -7464,57 +7469,57 @@
         <v>74</v>
       </c>
       <c r="D121" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E121" t="s">
+        <v>878</v>
+      </c>
+      <c r="F121" t="s">
+        <v>879</v>
+      </c>
+      <c r="G121" t="s">
         <v>880</v>
       </c>
-      <c r="F121" t="s">
+      <c r="H121" t="s">
         <v>881</v>
       </c>
-      <c r="G121" t="s">
+      <c r="I121" t="s">
         <v>882</v>
       </c>
-      <c r="H121" t="s">
+      <c r="J121" t="s">
         <v>883</v>
-      </c>
-      <c r="I121" t="s">
-        <v>884</v>
-      </c>
-      <c r="J121" t="s">
-        <v>885</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="B122" t="s">
         <v>11</v>
       </c>
       <c r="C122" t="s">
+        <v>885</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>886</v>
+      </c>
+      <c r="E122" s="2" t="s">
         <v>887</v>
       </c>
-      <c r="D122" s="3" t="s">
+      <c r="F122" s="2" t="s">
         <v>888</v>
       </c>
-      <c r="E122" s="2" t="s">
+      <c r="G122" s="3" t="s">
         <v>889</v>
       </c>
-      <c r="F122" s="2" t="s">
+      <c r="H122" s="3" t="s">
         <v>890</v>
       </c>
-      <c r="G122" s="3" t="s">
+      <c r="I122" s="3" t="s">
         <v>891</v>
       </c>
-      <c r="H122" s="3" t="s">
+      <c r="J122" s="3" t="s">
         <v>892</v>
-      </c>
-      <c r="I122" s="3" t="s">
-        <v>893</v>
-      </c>
-      <c r="J122" s="3" t="s">
-        <v>894</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.25">
@@ -7525,28 +7530,28 @@
         <v>21</v>
       </c>
       <c r="C123" t="s">
+        <v>893</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>894</v>
+      </c>
+      <c r="E123" s="3" t="s">
         <v>895</v>
       </c>
-      <c r="D123" s="3" t="s">
+      <c r="F123" s="3" t="s">
         <v>896</v>
       </c>
-      <c r="E123" s="3" t="s">
+      <c r="G123" s="3" t="s">
         <v>897</v>
       </c>
-      <c r="F123" s="3" t="s">
+      <c r="H123" s="3" t="s">
         <v>898</v>
       </c>
-      <c r="G123" s="3" t="s">
+      <c r="I123" s="3" t="s">
         <v>899</v>
       </c>
-      <c r="H123" s="3" t="s">
+      <c r="J123" s="3" t="s">
         <v>900</v>
-      </c>
-      <c r="I123" s="3" t="s">
-        <v>901</v>
-      </c>
-      <c r="J123" s="3" t="s">
-        <v>902</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.25">
@@ -7557,28 +7562,28 @@
         <v>30</v>
       </c>
       <c r="C124" t="s">
+        <v>901</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>902</v>
+      </c>
+      <c r="E124" s="2" t="s">
         <v>903</v>
       </c>
-      <c r="D124" s="2" t="s">
+      <c r="F124" s="2" t="s">
         <v>904</v>
       </c>
-      <c r="E124" s="2" t="s">
+      <c r="G124" s="2" t="s">
         <v>905</v>
       </c>
-      <c r="F124" s="2" t="s">
+      <c r="H124" s="2" t="s">
         <v>906</v>
       </c>
-      <c r="G124" s="2" t="s">
+      <c r="I124" s="2" t="s">
         <v>907</v>
       </c>
-      <c r="H124" s="2" t="s">
+      <c r="J124" s="2" t="s">
         <v>908</v>
-      </c>
-      <c r="I124" s="2" t="s">
-        <v>909</v>
-      </c>
-      <c r="J124" s="2" t="s">
-        <v>910</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.25">
@@ -7589,28 +7594,28 @@
         <v>39</v>
       </c>
       <c r="C125" t="s">
+        <v>909</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>910</v>
+      </c>
+      <c r="E125" s="3" t="s">
         <v>911</v>
       </c>
-      <c r="D125" s="3" t="s">
+      <c r="F125" s="3" t="s">
         <v>912</v>
       </c>
-      <c r="E125" s="3" t="s">
+      <c r="G125" s="3" t="s">
         <v>913</v>
       </c>
-      <c r="F125" s="3" t="s">
+      <c r="H125" s="2" t="s">
         <v>914</v>
       </c>
-      <c r="G125" s="3" t="s">
+      <c r="I125" s="2" t="s">
         <v>915</v>
       </c>
-      <c r="H125" s="2" t="s">
+      <c r="J125" s="2" t="s">
         <v>916</v>
-      </c>
-      <c r="I125" s="2" t="s">
-        <v>917</v>
-      </c>
-      <c r="J125" s="2" t="s">
-        <v>918</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.25">
@@ -7621,28 +7626,28 @@
         <v>48</v>
       </c>
       <c r="C126" t="s">
+        <v>917</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>918</v>
+      </c>
+      <c r="E126" s="3" t="s">
         <v>919</v>
       </c>
-      <c r="D126" s="3" t="s">
+      <c r="F126" s="3" t="s">
         <v>920</v>
       </c>
-      <c r="E126" s="3" t="s">
+      <c r="G126" s="2" t="s">
         <v>921</v>
       </c>
-      <c r="F126" s="3" t="s">
+      <c r="H126" s="2" t="s">
         <v>922</v>
       </c>
-      <c r="G126" s="2" t="s">
+      <c r="I126" s="2" t="s">
         <v>923</v>
       </c>
-      <c r="H126" s="2" t="s">
+      <c r="J126" s="2" t="s">
         <v>924</v>
-      </c>
-      <c r="I126" s="2" t="s">
-        <v>925</v>
-      </c>
-      <c r="J126" s="2" t="s">
-        <v>926</v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.25">
@@ -7653,28 +7658,28 @@
         <v>57</v>
       </c>
       <c r="C127" t="s">
+        <v>925</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>926</v>
+      </c>
+      <c r="E127" s="2" t="s">
         <v>927</v>
       </c>
-      <c r="D127" s="2" t="s">
+      <c r="F127" s="2" t="s">
         <v>928</v>
       </c>
-      <c r="E127" s="2" t="s">
+      <c r="G127" s="2" t="s">
         <v>929</v>
       </c>
-      <c r="F127" s="2" t="s">
+      <c r="H127" s="2" t="s">
         <v>930</v>
       </c>
-      <c r="G127" s="2" t="s">
+      <c r="I127" s="2" t="s">
         <v>931</v>
       </c>
-      <c r="H127" s="2" t="s">
+      <c r="J127" s="2" t="s">
         <v>932</v>
-      </c>
-      <c r="I127" s="2" t="s">
-        <v>933</v>
-      </c>
-      <c r="J127" s="2" t="s">
-        <v>934</v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.25">
@@ -7685,7 +7690,7 @@
         <v>66</v>
       </c>
       <c r="C128" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="D128" t="s">
         <v>193</v>
@@ -7703,7 +7708,7 @@
         <v>194</v>
       </c>
       <c r="I128" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="J128" t="s">
         <v>70</v>
@@ -7720,57 +7725,57 @@
         <v>74</v>
       </c>
       <c r="D129" t="s">
+        <v>933</v>
+      </c>
+      <c r="E129" t="s">
+        <v>934</v>
+      </c>
+      <c r="F129" t="s">
         <v>935</v>
       </c>
-      <c r="E129" t="s">
+      <c r="G129" t="s">
         <v>936</v>
       </c>
-      <c r="F129" t="s">
+      <c r="H129" t="s">
         <v>937</v>
       </c>
-      <c r="G129" t="s">
+      <c r="I129" t="s">
         <v>938</v>
       </c>
-      <c r="H129" t="s">
+      <c r="J129" t="s">
         <v>939</v>
-      </c>
-      <c r="I129" t="s">
-        <v>940</v>
-      </c>
-      <c r="J129" t="s">
-        <v>941</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="B130" t="s">
         <v>11</v>
       </c>
       <c r="C130" t="s">
+        <v>941</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>942</v>
+      </c>
+      <c r="E130" s="3" t="s">
         <v>943</v>
       </c>
-      <c r="D130" s="3" t="s">
+      <c r="F130" s="3" t="s">
         <v>944</v>
       </c>
-      <c r="E130" s="3" t="s">
+      <c r="G130" s="3" t="s">
         <v>945</v>
       </c>
-      <c r="F130" s="3" t="s">
+      <c r="H130" s="3" t="s">
         <v>946</v>
       </c>
-      <c r="G130" s="3" t="s">
+      <c r="I130" s="3" t="s">
         <v>947</v>
       </c>
-      <c r="H130" s="3" t="s">
+      <c r="J130" s="3" t="s">
         <v>948</v>
-      </c>
-      <c r="I130" s="3" t="s">
-        <v>949</v>
-      </c>
-      <c r="J130" s="3" t="s">
-        <v>950</v>
       </c>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.25">
@@ -7781,28 +7786,28 @@
         <v>21</v>
       </c>
       <c r="C131" t="s">
+        <v>949</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>950</v>
+      </c>
+      <c r="E131" s="3" t="s">
         <v>951</v>
       </c>
-      <c r="D131" s="2" t="s">
+      <c r="F131" s="3" t="s">
         <v>952</v>
       </c>
-      <c r="E131" s="3" t="s">
+      <c r="G131" s="3" t="s">
         <v>953</v>
       </c>
-      <c r="F131" s="3" t="s">
+      <c r="H131" s="3" t="s">
         <v>954</v>
       </c>
-      <c r="G131" s="3" t="s">
+      <c r="I131" s="3" t="s">
         <v>955</v>
       </c>
-      <c r="H131" s="3" t="s">
+      <c r="J131" s="3" t="s">
         <v>956</v>
-      </c>
-      <c r="I131" s="3" t="s">
-        <v>957</v>
-      </c>
-      <c r="J131" s="3" t="s">
-        <v>958</v>
       </c>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.25">
@@ -7813,28 +7818,28 @@
         <v>30</v>
       </c>
       <c r="C132" t="s">
+        <v>957</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>958</v>
+      </c>
+      <c r="E132" s="3" t="s">
         <v>959</v>
       </c>
-      <c r="D132" s="2" t="s">
+      <c r="F132" s="3" t="s">
         <v>960</v>
       </c>
-      <c r="E132" s="3" t="s">
+      <c r="G132" s="3" t="s">
         <v>961</v>
       </c>
-      <c r="F132" s="3" t="s">
+      <c r="H132" s="3" t="s">
         <v>962</v>
       </c>
-      <c r="G132" s="3" t="s">
+      <c r="I132" s="3" t="s">
         <v>963</v>
       </c>
-      <c r="H132" s="3" t="s">
+      <c r="J132" s="3" t="s">
         <v>964</v>
-      </c>
-      <c r="I132" s="3" t="s">
-        <v>965</v>
-      </c>
-      <c r="J132" s="3" t="s">
-        <v>966</v>
       </c>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.25">
@@ -7845,28 +7850,28 @@
         <v>39</v>
       </c>
       <c r="C133" t="s">
+        <v>965</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>966</v>
+      </c>
+      <c r="E133" s="3" t="s">
         <v>967</v>
       </c>
-      <c r="D133" s="3" t="s">
+      <c r="F133" s="3" t="s">
         <v>968</v>
       </c>
-      <c r="E133" s="3" t="s">
+      <c r="G133" s="3" t="s">
         <v>969</v>
       </c>
-      <c r="F133" s="3" t="s">
+      <c r="H133" s="3" t="s">
         <v>970</v>
       </c>
-      <c r="G133" s="3" t="s">
+      <c r="I133" s="3" t="s">
         <v>971</v>
       </c>
-      <c r="H133" s="3" t="s">
+      <c r="J133" s="3" t="s">
         <v>972</v>
-      </c>
-      <c r="I133" s="3" t="s">
-        <v>973</v>
-      </c>
-      <c r="J133" s="3" t="s">
-        <v>974</v>
       </c>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.25">
@@ -7877,28 +7882,28 @@
         <v>48</v>
       </c>
       <c r="C134" t="s">
+        <v>973</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>974</v>
+      </c>
+      <c r="E134" s="2" t="s">
         <v>975</v>
       </c>
-      <c r="D134" s="2" t="s">
+      <c r="F134" s="2" t="s">
         <v>976</v>
       </c>
-      <c r="E134" s="2" t="s">
+      <c r="G134" s="3" t="s">
         <v>977</v>
       </c>
-      <c r="F134" s="2" t="s">
+      <c r="H134" s="3" t="s">
         <v>978</v>
       </c>
-      <c r="G134" s="3" t="s">
+      <c r="I134" s="3" t="s">
         <v>979</v>
       </c>
-      <c r="H134" s="3" t="s">
+      <c r="J134" s="3" t="s">
         <v>980</v>
-      </c>
-      <c r="I134" s="3" t="s">
-        <v>981</v>
-      </c>
-      <c r="J134" s="3" t="s">
-        <v>982</v>
       </c>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.25">
@@ -7909,28 +7914,28 @@
         <v>57</v>
       </c>
       <c r="C135" t="s">
+        <v>981</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>982</v>
+      </c>
+      <c r="E135" t="s">
         <v>983</v>
       </c>
-      <c r="D135" s="2" t="s">
+      <c r="F135" s="3" t="s">
         <v>984</v>
       </c>
-      <c r="E135" t="s">
+      <c r="G135" s="3" t="s">
         <v>985</v>
       </c>
-      <c r="F135" s="3" t="s">
+      <c r="H135" s="3" t="s">
         <v>986</v>
       </c>
-      <c r="G135" s="3" t="s">
+      <c r="I135" s="3" t="s">
         <v>987</v>
       </c>
-      <c r="H135" s="3" t="s">
+      <c r="J135" s="3" t="s">
         <v>988</v>
-      </c>
-      <c r="I135" s="3" t="s">
-        <v>989</v>
-      </c>
-      <c r="J135" s="3" t="s">
-        <v>990</v>
       </c>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.25">
@@ -7944,25 +7949,25 @@
         <v>257</v>
       </c>
       <c r="D136" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E136" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F136" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G136" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H136" t="s">
         <v>133</v>
       </c>
       <c r="I136" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="J136" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.25">
@@ -7976,57 +7981,57 @@
         <v>74</v>
       </c>
       <c r="D137" t="s">
+        <v>989</v>
+      </c>
+      <c r="E137" t="s">
+        <v>990</v>
+      </c>
+      <c r="F137" t="s">
         <v>991</v>
       </c>
-      <c r="E137" t="s">
+      <c r="G137" t="s">
         <v>992</v>
       </c>
-      <c r="F137" t="s">
+      <c r="H137" t="s">
         <v>993</v>
       </c>
-      <c r="G137" t="s">
+      <c r="I137" t="s">
         <v>994</v>
       </c>
-      <c r="H137" t="s">
+      <c r="J137" t="s">
         <v>995</v>
-      </c>
-      <c r="I137" t="s">
-        <v>996</v>
-      </c>
-      <c r="J137" t="s">
-        <v>997</v>
       </c>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="B138" t="s">
         <v>11</v>
       </c>
       <c r="C138" t="s">
+        <v>997</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>998</v>
+      </c>
+      <c r="E138" s="2" t="s">
         <v>999</v>
       </c>
-      <c r="D138" s="2" t="s">
+      <c r="F138" s="2" t="s">
         <v>1000</v>
       </c>
-      <c r="E138" s="2" t="s">
+      <c r="G138" s="2" t="s">
         <v>1001</v>
       </c>
-      <c r="F138" s="2" t="s">
+      <c r="H138" s="2" t="s">
         <v>1002</v>
       </c>
-      <c r="G138" s="2" t="s">
+      <c r="I138" s="2" t="s">
         <v>1003</v>
       </c>
-      <c r="H138" s="2" t="s">
+      <c r="J138" s="2" t="s">
         <v>1004</v>
-      </c>
-      <c r="I138" s="2" t="s">
-        <v>1005</v>
-      </c>
-      <c r="J138" s="2" t="s">
-        <v>1006</v>
       </c>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.25">
@@ -8037,28 +8042,28 @@
         <v>21</v>
       </c>
       <c r="C139" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D139" s="2" t="s">
+        <v>1006</v>
+      </c>
+      <c r="E139" s="3" t="s">
         <v>1007</v>
       </c>
-      <c r="D139" s="2" t="s">
+      <c r="F139" s="3" t="s">
         <v>1008</v>
       </c>
-      <c r="E139" s="3" t="s">
+      <c r="G139" s="2" t="s">
         <v>1009</v>
       </c>
-      <c r="F139" s="3" t="s">
+      <c r="H139" s="2" t="s">
         <v>1010</v>
       </c>
-      <c r="G139" s="2" t="s">
+      <c r="I139" s="2" t="s">
         <v>1011</v>
       </c>
-      <c r="H139" s="2" t="s">
+      <c r="J139" s="2" t="s">
         <v>1012</v>
-      </c>
-      <c r="I139" s="2" t="s">
-        <v>1013</v>
-      </c>
-      <c r="J139" s="2" t="s">
-        <v>1014</v>
       </c>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.25">
@@ -8069,28 +8074,28 @@
         <v>30</v>
       </c>
       <c r="C140" t="s">
+        <v>1013</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>1014</v>
+      </c>
+      <c r="E140" s="2" t="s">
         <v>1015</v>
       </c>
-      <c r="D140" s="2" t="s">
+      <c r="F140" s="2" t="s">
         <v>1016</v>
       </c>
-      <c r="E140" s="2" t="s">
+      <c r="G140" s="2" t="s">
         <v>1017</v>
       </c>
-      <c r="F140" s="2" t="s">
+      <c r="H140" s="2" t="s">
         <v>1018</v>
       </c>
-      <c r="G140" s="2" t="s">
+      <c r="I140" s="2" t="s">
         <v>1019</v>
       </c>
-      <c r="H140" s="2" t="s">
+      <c r="J140" s="2" t="s">
         <v>1020</v>
-      </c>
-      <c r="I140" s="2" t="s">
-        <v>1021</v>
-      </c>
-      <c r="J140" s="2" t="s">
-        <v>1022</v>
       </c>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.25">
@@ -8101,28 +8106,28 @@
         <v>39</v>
       </c>
       <c r="C141" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E141" s="2" t="s">
         <v>1023</v>
       </c>
-      <c r="D141" s="2" t="s">
+      <c r="F141" s="2" t="s">
         <v>1024</v>
       </c>
-      <c r="E141" s="2" t="s">
+      <c r="G141" s="2" t="s">
         <v>1025</v>
       </c>
-      <c r="F141" s="2" t="s">
+      <c r="H141" s="2" t="s">
         <v>1026</v>
       </c>
-      <c r="G141" s="2" t="s">
+      <c r="I141" s="2" t="s">
         <v>1027</v>
       </c>
-      <c r="H141" s="2" t="s">
+      <c r="J141" s="2" t="s">
         <v>1028</v>
-      </c>
-      <c r="I141" s="2" t="s">
-        <v>1029</v>
-      </c>
-      <c r="J141" s="2" t="s">
-        <v>1030</v>
       </c>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.25">
@@ -8133,28 +8138,28 @@
         <v>48</v>
       </c>
       <c r="C142" t="s">
+        <v>1029</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>1030</v>
+      </c>
+      <c r="E142" s="2" t="s">
         <v>1031</v>
       </c>
-      <c r="D142" s="2" t="s">
+      <c r="F142" s="2" t="s">
         <v>1032</v>
       </c>
-      <c r="E142" s="2" t="s">
+      <c r="G142" s="2" t="s">
         <v>1033</v>
       </c>
-      <c r="F142" s="2" t="s">
+      <c r="H142" s="2" t="s">
         <v>1034</v>
       </c>
-      <c r="G142" s="2" t="s">
+      <c r="I142" s="2" t="s">
         <v>1035</v>
       </c>
-      <c r="H142" s="2" t="s">
+      <c r="J142" s="2" t="s">
         <v>1036</v>
-      </c>
-      <c r="I142" s="2" t="s">
-        <v>1037</v>
-      </c>
-      <c r="J142" s="2" t="s">
-        <v>1038</v>
       </c>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.25">
@@ -8165,28 +8170,28 @@
         <v>57</v>
       </c>
       <c r="C143" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>1038</v>
+      </c>
+      <c r="E143" s="2" t="s">
         <v>1039</v>
       </c>
-      <c r="D143" s="2" t="s">
+      <c r="F143" s="2" t="s">
         <v>1040</v>
       </c>
-      <c r="E143" s="2" t="s">
+      <c r="G143" s="2" t="s">
         <v>1041</v>
       </c>
-      <c r="F143" s="2" t="s">
+      <c r="H143" s="2" t="s">
         <v>1042</v>
       </c>
-      <c r="G143" s="2" t="s">
+      <c r="I143" s="2" t="s">
         <v>1043</v>
       </c>
-      <c r="H143" s="2" t="s">
+      <c r="J143" s="2" t="s">
         <v>1044</v>
-      </c>
-      <c r="I143" s="2" t="s">
-        <v>1045</v>
-      </c>
-      <c r="J143" s="2" t="s">
-        <v>1046</v>
       </c>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.25">
@@ -8197,7 +8202,7 @@
         <v>66</v>
       </c>
       <c r="C144" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="D144" t="s">
         <v>136</v>
@@ -8206,13 +8211,13 @@
         <v>69</v>
       </c>
       <c r="F144" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="G144" t="s">
         <v>72</v>
       </c>
       <c r="H144" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I144" t="s">
         <v>194</v>
@@ -8232,25 +8237,25 @@
         <v>74</v>
       </c>
       <c r="D145" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E145" t="s">
+        <v>1047</v>
+      </c>
+      <c r="F145" t="s">
         <v>1048</v>
       </c>
-      <c r="E145" t="s">
+      <c r="G145" t="s">
         <v>1049</v>
       </c>
-      <c r="F145" t="s">
+      <c r="H145" t="s">
         <v>1050</v>
       </c>
-      <c r="G145" t="s">
+      <c r="I145" t="s">
         <v>1051</v>
       </c>
-      <c r="H145" t="s">
-        <v>1052</v>
-      </c>
-      <c r="I145" t="s">
-        <v>1053</v>
-      </c>
       <c r="J145" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.25">
@@ -8258,7 +8263,7 @@
         <v>20</v>
       </c>
       <c r="B146" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="C146" s="4">
         <v>5.8888888888888893</v>
@@ -8290,31 +8295,31 @@
         <v>20</v>
       </c>
       <c r="B147" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="C147" t="s">
         <v>74</v>
       </c>
       <c r="D147" t="s">
+        <v>1054</v>
+      </c>
+      <c r="E147" t="s">
+        <v>1055</v>
+      </c>
+      <c r="F147" t="s">
         <v>1056</v>
       </c>
-      <c r="E147" t="s">
+      <c r="G147" t="s">
         <v>1057</v>
       </c>
-      <c r="F147" t="s">
+      <c r="H147" t="s">
         <v>1058</v>
       </c>
-      <c r="G147" t="s">
+      <c r="I147" t="s">
+        <v>547</v>
+      </c>
+      <c r="J147" t="s">
         <v>1059</v>
-      </c>
-      <c r="H147" t="s">
-        <v>1060</v>
-      </c>
-      <c r="I147" t="s">
-        <v>548</v>
-      </c>
-      <c r="J147" t="s">
-        <v>1061</v>
       </c>
     </row>
   </sheetData>

</xml_diff>